<commit_message>
Update template to include originator information
</commit_message>
<xml_diff>
--- a/sepacetamol/static/sepa-xml-template.xlsx
+++ b/sepacetamol/static/sepa-xml-template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zaytsev/Documents/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77237867-B050-6E4F-AE11-FEF5DEDE0251}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE0BA34-F94F-2542-AEEB-F0068D31CCED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16260" xr2:uid="{251EE6FE-9347-D943-90D4-558197AE6232}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Transactions" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>Recipient name</t>
   </si>
@@ -47,12 +47,6 @@
     <t>Purpose</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
-    <t>CANCOM GmbH</t>
-  </si>
-  <si>
     <t>DE17 7204 0046 0112 9212 00</t>
   </si>
   <si>
@@ -60,6 +54,30 @@
   </si>
   <si>
     <t>Kdn. 1234567</t>
+  </si>
+  <si>
+    <t>Reference (optional)</t>
+  </si>
+  <si>
+    <t>Sender name</t>
+  </si>
+  <si>
+    <t>DE02120300000000202051</t>
+  </si>
+  <si>
+    <t>Sender IBAN</t>
+  </si>
+  <si>
+    <t>CANCOM1 GmbH</t>
+  </si>
+  <si>
+    <t>CANCOM2 GmbH</t>
+  </si>
+  <si>
+    <t>CANCOM3 GmbH</t>
+  </si>
+  <si>
+    <t>honeymeets continuity GmbH</t>
   </si>
 </sst>
 </file>
@@ -95,13 +113,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -115,16 +138,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E1AC855C-897B-2942-A524-C2C082082DA5}" name="Table2" displayName="Table2" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4" xr:uid="{B5FC1433-D771-B148-A028-0885054FA8F7}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E1AC855C-897B-2942-A524-C2C082082DA5}" name="Table2" displayName="Table2" ref="A3:E30" totalsRowShown="0">
+  <autoFilter ref="A3:E30" xr:uid="{B5FC1433-D771-B148-A028-0885054FA8F7}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{75528291-B420-354F-BC7D-5095D394A607}" name="Recipient name"/>
     <tableColumn id="2" xr3:uid="{86A6B908-A4B7-C748-87F9-6D410449287F}" name="Recipient IBAN"/>
-    <tableColumn id="3" xr3:uid="{F68029C1-E593-224B-A6EB-CA2FBD7AA937}" name="Amount"/>
+    <tableColumn id="3" xr3:uid="{F68029C1-E593-224B-A6EB-CA2FBD7AA937}" name="Amount" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{B931F3E8-A794-984D-8317-F4B325A494F6}" name="Purpose"/>
-    <tableColumn id="5" xr3:uid="{816F685F-5530-0049-AC67-2B4F4302567F}" name="Reference"/>
+    <tableColumn id="5" xr3:uid="{816F685F-5530-0049-AC67-2B4F4302567F}" name="Reference (optional)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1C6B5ACA-EC3C-1D45-87AA-628365D96A20}" name="Table1" displayName="Table1" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{BFA7E51A-89B6-DD45-948E-E1092EA7D5E5}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{525BBD99-875E-5C45-A3B1-2D63571EAA13}" name="Sender name"/>
+    <tableColumn id="2" xr3:uid="{64F2A3E0-8331-7E4C-81E7-2BE4C940CD71}" name="Sender IBAN"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -425,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37FD2542-A6C1-4E4F-9175-994A48609C5C}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,76 +476,162 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>123.45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>123.45</v>
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
         <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
         <v>123.45</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>123.12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>